<commit_message>
update for intermediate vs rookie
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppDev\code\trap-scoring\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF163FA4-6F83-4042-ACF8-D97AFC5646BF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7080A4C1-5CAC-4FC1-A7FB-3E62EABFDDD8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="40">
   <si>
     <t>EventId</t>
   </si>
@@ -248,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -263,6 +263,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,9 +699,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -743,48 +744,135 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" customWidth="1"/>
+    <col min="21" max="24" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="61.5" x14ac:dyDescent="0.9">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:24" ht="61.5" x14ac:dyDescent="0.9">
+      <c r="A1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="D1" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="P1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="M1" s="5" t="s">
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="U1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="5"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X2" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="U1:X1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -792,122 +880,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:T2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.5703125" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" ht="61.5" x14ac:dyDescent="0.9">
-      <c r="A1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="E1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="I1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="M1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="Q1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="R1" s="5"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" t="s">
-        <v>38</v>
-      </c>
-      <c r="N2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" t="s">
-        <v>7</v>
-      </c>
-      <c r="T2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -915,50 +888,58 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" customWidth="1"/>
+    <col min="21" max="24" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="61.5" x14ac:dyDescent="0.9">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:24" ht="61.5" x14ac:dyDescent="0.9">
+      <c r="A1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="I1" s="5" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="M1" s="5" t="s">
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="P1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="U1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="5"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -971,56 +952,198 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="K2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="L2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="M2" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="N2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="P2" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="Q2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R2" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="S2" t="s">
-        <v>7</v>
-      </c>
-      <c r="T2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X2" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="U1:X1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" customWidth="1"/>
+    <col min="21" max="24" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="61.5" x14ac:dyDescent="0.9">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="F1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="K1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="P1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="U1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upload new excel files
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -8,18 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppDev\code\trap-scoring\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7080A4C1-5CAC-4FC1-A7FB-3E62EABFDDD8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4199AAD8-130B-400E-9FAC-6A834DA027DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="18420" windowHeight="11745" tabRatio="623"/>
   </bookViews>
   <sheets>
     <sheet name="Clean Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Senior" sheetId="2" r:id="rId2"/>
-    <sheet name="Intermediate Rookie" sheetId="3" r:id="rId3"/>
-    <sheet name="Individual Men" sheetId="4" r:id="rId4"/>
-    <sheet name="Individual Women" sheetId="6" r:id="rId5"/>
+    <sheet name="Team-Senior" sheetId="2" r:id="rId2"/>
+    <sheet name="Team-Intermediate" sheetId="7" r:id="rId3"/>
+    <sheet name="Team-Rookie" sheetId="8" r:id="rId4"/>
+    <sheet name="Individual-Men" sheetId="4" r:id="rId5"/>
+    <sheet name="Individual-Ladies" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">#N/A</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5">#N/A</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4">#N/A</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Clean Data'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">'Individual-Ladies'!$1:$13</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">'Individual-Men'!$1:$13</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Team-Intermediate'!$1:$12</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'Team-Rookie'!$1:$12</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Team-Senior'!$1:$12</definedName>
+  </definedNames>
+  <calcPr calcId="179017" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -59,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
   <si>
     <t>EventId</t>
   </si>
@@ -179,13 +191,31 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>As of: 2/12/2019</t>
+  </si>
+  <si>
+    <t>2019 State League Standings: Intermediate Division</t>
+  </si>
+  <si>
+    <t>2019 State League Standings: Senior Division</t>
+  </si>
+  <si>
+    <t>2019 State League Standings: Rookie Division</t>
+  </si>
+  <si>
+    <t>2019 State League Standings: Individual Men</t>
+  </si>
+  <si>
+    <t>2019 State League Standings: Individual Ladies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,7 +251,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="48"/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -236,7 +280,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -244,11 +288,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -262,10 +317,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -281,6 +345,771 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2061" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D5FFDA8-2C52-4885-BA48-6D4F3EFF257B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="276225" y="209550"/>
+          <a:ext cx="3438525" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1704975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2314575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2062" name="Picture 2" descr="Iowa Department of Natural Resources">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A706F73A-BE2A-4A25-9021-BCC3D6CAB914}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5391150" y="142875"/>
+          <a:ext cx="4048125" cy="790575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3085" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76182160-6239-4FDE-BD1B-28BF40C1AB59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="276225" y="209550"/>
+          <a:ext cx="3438525" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1704975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2314575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3086" name="Picture 4" descr="Iowa Department of Natural Resources">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1D91790-7565-4730-8657-7B03EA23A3DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5391150" y="142875"/>
+          <a:ext cx="4048125" cy="790575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4109" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{322DFFE4-1DAC-4FDD-A261-F8943DCCFF44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="276225" y="209550"/>
+          <a:ext cx="3438525" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1704975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2314575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4110" name="Picture 2" descr="Iowa Department of Natural Resources">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56435814-7278-43B6-93A1-9DEC2F1BCB10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5391150" y="142875"/>
+          <a:ext cx="4048125" cy="790575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1819275</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5153" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62718721-CE5C-49E8-B351-D810BED232A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="276225" y="209550"/>
+          <a:ext cx="3552825" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1704975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5154" name="Picture 4" descr="Iowa Department of Natural Resources">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DEFC316-2B97-4878-A29B-05BC26C3703E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4705350" y="142875"/>
+          <a:ext cx="4143375" cy="790575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1200150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6178" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B64E54AA-3A26-4CD3-A65B-37E640819579}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="276225" y="209550"/>
+          <a:ext cx="3495675" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1704975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6179" name="Picture 2" descr="Iowa Department of Natural Resources">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D33D0ABF-5292-4901-9FA2-88C4BA903B6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5800725" y="142875"/>
+          <a:ext cx="3981450" cy="790575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -583,9 +1412,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AG1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:33" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -689,461 +1526,680 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AG1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:N1"/>
+  <sheetPr codeName="Sheet2">
+    <tabColor theme="9" tint="0.79998168889431442"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B9:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" customWidth="1"/>
+    <col min="11" max="11" width="35.7109375" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" customWidth="1"/>
+    <col min="14" max="14" width="35.7109375" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="61.5" x14ac:dyDescent="0.9">
-      <c r="A1" s="5" t="s">
+    <row r="9" spans="2:14" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="B9" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B10" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" s="11" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="D1" s="5" t="s">
+      <c r="E12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="H12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="J1" s="5" t="s">
+      <c r="K12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="M1" s="5" t="s">
+      <c r="N12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="54" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:X2"/>
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" customWidth="1"/>
-    <col min="21" max="24" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="35.7109375" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" style="8" customWidth="1"/>
+    <col min="14" max="14" width="35.7109375" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="61.5" x14ac:dyDescent="0.9">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+      <c r="F1"/>
+      <c r="I1"/>
+      <c r="L1"/>
+      <c r="O1"/>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C2"/>
+      <c r="F2"/>
+      <c r="I2"/>
+      <c r="L2"/>
+      <c r="O2"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C3"/>
+      <c r="F3"/>
+      <c r="I3"/>
+      <c r="L3"/>
+      <c r="O3"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C4"/>
+      <c r="F4"/>
+      <c r="I4"/>
+      <c r="L4"/>
+      <c r="O4"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C5"/>
+      <c r="F5"/>
+      <c r="I5"/>
+      <c r="L5"/>
+      <c r="O5"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C6"/>
+      <c r="F6"/>
+      <c r="I6"/>
+      <c r="L6"/>
+      <c r="O6"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C7"/>
+      <c r="F7"/>
+      <c r="I7"/>
+      <c r="L7"/>
+      <c r="O7"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C8"/>
+      <c r="F8"/>
+      <c r="I8"/>
+      <c r="L8"/>
+      <c r="O8"/>
+    </row>
+    <row r="9" spans="2:15" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="B9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9"/>
+      <c r="F9"/>
+      <c r="I9"/>
+      <c r="L9"/>
+      <c r="O9"/>
+    </row>
+    <row r="10" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10"/>
+      <c r="F10"/>
+      <c r="I10"/>
+      <c r="L10"/>
+      <c r="O10"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C11"/>
+      <c r="F11"/>
+      <c r="I11"/>
+      <c r="L11"/>
+      <c r="O11"/>
+    </row>
+    <row r="12" spans="2:15" s="11" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="E12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="K1" s="6" t="s">
+      <c r="H12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="P1" s="6" t="s">
+      <c r="K12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="U1" s="6" t="s">
+      <c r="N12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>39</v>
-      </c>
-      <c r="R2" t="s">
-        <v>7</v>
-      </c>
-      <c r="S2" t="s">
-        <v>9</v>
-      </c>
-      <c r="U2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" t="s">
-        <v>7</v>
-      </c>
-      <c r="X2" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="U1:X1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="53" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:X2"/>
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" customWidth="1"/>
-    <col min="21" max="24" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="35.7109375" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" style="8" customWidth="1"/>
+    <col min="14" max="14" width="35.7109375" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="61.5" x14ac:dyDescent="0.9">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+      <c r="F1"/>
+      <c r="I1"/>
+      <c r="L1"/>
+      <c r="O1"/>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C2"/>
+      <c r="F2"/>
+      <c r="I2"/>
+      <c r="L2"/>
+      <c r="O2"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C3"/>
+      <c r="F3"/>
+      <c r="I3"/>
+      <c r="L3"/>
+      <c r="O3"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C4"/>
+      <c r="F4"/>
+      <c r="I4"/>
+      <c r="L4"/>
+      <c r="O4"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C5"/>
+      <c r="F5"/>
+      <c r="I5"/>
+      <c r="L5"/>
+      <c r="O5"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C6"/>
+      <c r="F6"/>
+      <c r="I6"/>
+      <c r="L6"/>
+      <c r="O6"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C7"/>
+      <c r="F7"/>
+      <c r="I7"/>
+      <c r="L7"/>
+      <c r="O7"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C8"/>
+      <c r="F8"/>
+      <c r="I8"/>
+      <c r="L8"/>
+      <c r="O8"/>
+    </row>
+    <row r="9" spans="2:15" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="B9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9"/>
+      <c r="F9"/>
+      <c r="I9"/>
+      <c r="L9"/>
+      <c r="O9"/>
+    </row>
+    <row r="10" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10"/>
+      <c r="F10"/>
+      <c r="I10"/>
+      <c r="L10"/>
+      <c r="O10"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C11"/>
+      <c r="F11"/>
+      <c r="I11"/>
+      <c r="L11"/>
+      <c r="O11"/>
+    </row>
+    <row r="12" spans="2:15" s="11" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="E12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="K1" s="6" t="s">
+      <c r="H12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="P1" s="6" t="s">
+      <c r="K12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="U1" s="6" t="s">
+      <c r="N12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>39</v>
-      </c>
-      <c r="R2" t="s">
-        <v>7</v>
-      </c>
-      <c r="S2" t="s">
-        <v>9</v>
-      </c>
-      <c r="U2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" t="s">
-        <v>7</v>
-      </c>
-      <c r="X2" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="U1:X1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="53" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X2"/>
+  <sheetPr codeName="Sheet4">
+    <tabColor theme="5" tint="0.79998168889431442"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:T13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" style="7" customWidth="1"/>
+    <col min="12" max="12" width="35.7109375" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="35.7109375" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" customWidth="1"/>
+    <col min="18" max="18" width="19.7109375" customWidth="1"/>
+    <col min="19" max="19" width="6.7109375" style="7" customWidth="1"/>
+    <col min="20" max="20" width="35.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+      <c r="G1"/>
+      <c r="K1"/>
+      <c r="O1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C2"/>
+      <c r="G2"/>
+      <c r="K2"/>
+      <c r="O2"/>
+      <c r="S2"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C3"/>
+      <c r="G3"/>
+      <c r="K3"/>
+      <c r="O3"/>
+      <c r="S3"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C4"/>
+      <c r="G4"/>
+      <c r="K4"/>
+      <c r="O4"/>
+      <c r="S4"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C5"/>
+      <c r="G5"/>
+      <c r="K5"/>
+      <c r="O5"/>
+      <c r="S5"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C6"/>
+      <c r="G6"/>
+      <c r="K6"/>
+      <c r="O6"/>
+      <c r="S6"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C7"/>
+      <c r="G7"/>
+      <c r="K7"/>
+      <c r="O7"/>
+      <c r="S7"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C8"/>
+      <c r="G8"/>
+      <c r="K8"/>
+      <c r="O8"/>
+      <c r="S8"/>
+    </row>
+    <row r="9" spans="2:20" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="B9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9"/>
+      <c r="G9"/>
+      <c r="K9"/>
+      <c r="O9"/>
+      <c r="S9"/>
+    </row>
+    <row r="10" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10"/>
+      <c r="G10"/>
+      <c r="K10"/>
+      <c r="O10"/>
+      <c r="S10"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C11"/>
+      <c r="G11"/>
+      <c r="K11"/>
+      <c r="O11"/>
+      <c r="S11"/>
+    </row>
+    <row r="12" spans="2:20" s="11" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="S13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="40" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="3" tint="0.79998168889431442"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:T13"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" customWidth="1"/>
-    <col min="21" max="24" width="13.5703125" customWidth="1"/>
+    <col min="15" max="15" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="61.5" x14ac:dyDescent="0.9">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+    </row>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C3"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C4"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C5"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C6"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C7"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C8"/>
+    </row>
+    <row r="9" spans="2:20" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="B9" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9"/>
+    </row>
+    <row r="10" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C11"/>
+    </row>
+    <row r="12" spans="2:20" s="11" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="F12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="K1" s="6" t="s">
+      <c r="J12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="P1" s="6" t="s">
+      <c r="N12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="U1" s="6" t="s">
+      <c r="R12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="13" spans="2:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="F13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="J13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L2" t="s">
+      <c r="K13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M2" t="s">
+      <c r="L13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="N13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="O13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="R2" t="s">
+      <c r="P13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="S2" t="s">
-        <v>9</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="R13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="V2" t="s">
+      <c r="S13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="W2" t="s">
+      <c r="T13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="X2" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="40" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rookies only display singles
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppDev\code\trap-scoring\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4199AAD8-130B-400E-9FAC-6A834DA027DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7F94FFC-9B46-49AC-B534-D54851827654}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="18420" windowHeight="11745" tabRatio="623"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="46">
   <si>
     <t>EventId</t>
   </si>
@@ -193,9 +193,6 @@
     <t>Score</t>
   </si>
   <si>
-    <t>As of: 2/12/2019</t>
-  </si>
-  <si>
     <t>2019 State League Standings: Intermediate Division</t>
   </si>
   <si>
@@ -209,6 +206,9 @@
   </si>
   <si>
     <t>2019 State League Standings: Individual Ladies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As of: </t>
   </si>
 </sst>
 </file>
@@ -364,10 +364,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2061" name="Picture 1">
+        <xdr:cNvPr id="2063" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D5FFDA8-2C52-4885-BA48-6D4F3EFF257B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DD195F0-6F4A-4778-A8FF-F72FCF55E475}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -438,10 +438,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2062" name="Picture 2" descr="Iowa Department of Natural Resources">
+        <xdr:cNvPr id="2064" name="Picture 2" descr="Iowa Department of Natural Resources">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A706F73A-BE2A-4A25-9021-BCC3D6CAB914}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5EF81FC-1CA7-4B79-A7D2-212709D76503}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -517,10 +517,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3085" name="Picture 3">
+        <xdr:cNvPr id="3087" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76182160-6239-4FDE-BD1B-28BF40C1AB59}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{206F3BD6-0697-41C7-A192-FA407972D1D6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -591,10 +591,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3086" name="Picture 4" descr="Iowa Department of Natural Resources">
+        <xdr:cNvPr id="3088" name="Picture 4" descr="Iowa Department of Natural Resources">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1D91790-7565-4730-8657-7B03EA23A3DA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7E730A8-D103-4260-9DB5-480E27259B7C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -670,10 +670,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4109" name="Picture 1">
+        <xdr:cNvPr id="4111" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{322DFFE4-1DAC-4FDD-A261-F8943DCCFF44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20E5C4A4-A17C-44C8-A211-E6EF8EA5EEED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -744,10 +744,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4110" name="Picture 2" descr="Iowa Department of Natural Resources">
+        <xdr:cNvPr id="4112" name="Picture 2" descr="Iowa Department of Natural Resources">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56435814-7278-43B6-93A1-9DEC2F1BCB10}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1E58F1D-AD3F-4D6B-A6F7-2E950CD0AFAE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -823,10 +823,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5153" name="Picture 3">
+        <xdr:cNvPr id="5155" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62718721-CE5C-49E8-B351-D810BED232A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0073C36C-F232-4169-8AD1-9D798C3FF305}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -897,10 +897,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5154" name="Picture 4" descr="Iowa Department of Natural Resources">
+        <xdr:cNvPr id="5156" name="Picture 4" descr="Iowa Department of Natural Resources">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DEFC316-2B97-4878-A29B-05BC26C3703E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{082770A5-07F0-4A40-9E91-F754DC08361E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -976,10 +976,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6178" name="Picture 1">
+        <xdr:cNvPr id="6180" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B64E54AA-3A26-4CD3-A65B-37E640819579}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EE43694-5565-457C-9880-18AEB8C70C3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1050,10 +1050,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6179" name="Picture 2" descr="Iowa Department of Natural Resources">
+        <xdr:cNvPr id="6181" name="Picture 2" descr="Iowa Department of Natural Resources">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D33D0ABF-5292-4901-9FA2-88C4BA903B6B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA20900B-C848-42ED-83AF-05D0940CD4BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1563,12 +1563,12 @@
   <sheetData>
     <row r="9" spans="2:14" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B9" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="2:14" s="11" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
@@ -1681,7 +1681,7 @@
     </row>
     <row r="9" spans="2:15" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B9" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9"/>
       <c r="F9"/>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="10" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C10"/>
       <c r="F10"/>
@@ -1816,7 +1816,7 @@
     </row>
     <row r="9" spans="2:15" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B9" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9"/>
       <c r="F9"/>
@@ -1826,7 +1826,7 @@
     </row>
     <row r="10" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C10"/>
       <c r="F10"/>
@@ -1844,18 +1844,6 @@
     <row r="12" spans="2:15" s="11" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B12" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="N12" s="11" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1960,7 +1948,7 @@
     </row>
     <row r="9" spans="2:20" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B9" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9"/>
       <c r="G9"/>
@@ -1970,7 +1958,7 @@
     </row>
     <row r="10" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C10"/>
       <c r="G10"/>
@@ -2117,13 +2105,13 @@
     </row>
     <row r="9" spans="2:20" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B9" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9"/>
     </row>
     <row r="10" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C10"/>
     </row>

</xml_diff>

<commit_message>
Added Fixed width column sizes
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -1,44 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppDev\code\trap-scoring\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9247733-24A3-4A00-A79F-0804647628E3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F942B243-8EF1-474C-BC41-00C8BDE17C71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="18240" windowHeight="7920" tabRatio="623"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="18240" windowHeight="7920" tabRatio="623" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clean Data" sheetId="1" r:id="rId1"/>
     <sheet name="Team-Senior" sheetId="2" r:id="rId2"/>
-    <sheet name="Team-Intermediate" sheetId="9" r:id="rId3"/>
-    <sheet name="Team-Rookie" sheetId="11" r:id="rId4"/>
+    <sheet name="Team-Intermediate" sheetId="14" r:id="rId3"/>
+    <sheet name="Team-Rookie" sheetId="15" r:id="rId4"/>
     <sheet name="Individual-Men" sheetId="4" r:id="rId5"/>
-    <sheet name="Individual-Ladies" sheetId="12" r:id="rId6"/>
+    <sheet name="Individual-Ladies" sheetId="16" r:id="rId6"/>
     <sheet name="Team-Individual-Scores" sheetId="13" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Clean Data'!$A$1:$W$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5">#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Individual-Ladies'!$A$13:$T$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Individual-Men'!$A$13:$T$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Team-Individual-Scores'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Team-Intermediate'!$A$1:$P$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Team-Rookie'!$A$1:$P$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Team-Senior'!$A$1:$P$12</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Clean Data'!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="5">'Individual-Ladies'!$1:$13</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'Individual-Men'!$1:$13</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Team-Intermediate'!$1:$12</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="3">'Team-Rookie'!$1:$12</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Team-Senior'!$1:$12</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Team-Intermediate'!$12:$12</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'Team-Rookie'!$12:$12</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Team-Senior'!$12:$12</definedName>
   </definedNames>
-  <calcPr calcId="179017" fullCalcOnLoad="1"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
   <si>
     <t>EventId</t>
   </si>
@@ -157,7 +160,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -280,8 +283,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>280988</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -355,7 +358,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2428875</xdr:colOff>
+      <xdr:colOff>2083593</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -501,23 +504,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1876425</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>280988</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7266" name="Picture 3" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E060C35-F025-4EC9-A9F3-0E3D5E83FBE2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13F7CE4F-753B-4DDA-9E61-3998DEBE4AFC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -540,8 +543,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11334750" y="209550"/>
-          <a:ext cx="1162050" cy="952500"/>
+          <a:off x="190500" y="209550"/>
+          <a:ext cx="3576638" cy="1028700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -575,23 +578,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1714500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2083593</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7267" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2" descr="Iowa Department of Natural Resources">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D13BF31D-7144-4D2C-8916-EBB5A91685FC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63B5BE74-514F-4F18-A16A-605CF8A98D47}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -614,8 +617,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="161925" y="200025"/>
-          <a:ext cx="3571875" cy="1038225"/>
+          <a:off x="5715000" y="142875"/>
+          <a:ext cx="4207668" cy="800100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -649,23 +652,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1695450</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>2428875</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1552575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7268" name="Picture 2" descr="Iowa Department of Natural Resources">
+        <xdr:cNvPr id="4" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A67C42B-579E-45EF-99D0-91326E168047}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6663856E-F654-4EB9-9BDB-1B1ABD809EF8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -688,8 +691,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5343525" y="161925"/>
-          <a:ext cx="4219575" cy="790575"/>
+          <a:off x="12077700" y="209550"/>
+          <a:ext cx="1152525" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -734,17 +737,17 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>280988</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9314" name="Picture 1">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A9C418D-FC10-4A7D-8257-3BAA535C4336}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E260745-D8AE-4701-9E3B-BD669E90D5CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -767,8 +770,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="200025" y="209550"/>
-          <a:ext cx="3571875" cy="1028700"/>
+          <a:off x="190500" y="209550"/>
+          <a:ext cx="3576638" cy="1028700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -803,22 +806,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1724025</xdr:colOff>
+      <xdr:colOff>1714500</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2438400</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>2083593</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9315" name="Picture 2" descr="Iowa Department of Natural Resources">
+        <xdr:cNvPr id="3" name="Picture 2" descr="Iowa Department of Natural Resources">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EC07843-82A6-4C25-93E2-830DD7CBBFCA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87AA494B-BE5B-4CD1-8DD0-69B92D43E4D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -841,8 +844,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5381625" y="161925"/>
-          <a:ext cx="4200525" cy="790575"/>
+          <a:off x="5715000" y="142875"/>
+          <a:ext cx="4207668" cy="800100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -877,22 +880,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1552575</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9316" name="Picture 3" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
+        <xdr:cNvPr id="4" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D8B78F8-6707-48DC-8CC8-2C4A612A56C1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A1E53A0-3DAF-41EB-99B2-273277619DB4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -915,8 +918,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10972800" y="190500"/>
-          <a:ext cx="1162050" cy="962025"/>
+          <a:off x="12077700" y="209550"/>
+          <a:ext cx="1152525" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -962,7 +965,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1828800</xdr:colOff>
+      <xdr:colOff>1293018</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1035,8 +1038,8 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2640806</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
@@ -1189,16 +1192,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1828800</xdr:colOff>
+      <xdr:colOff>1293018</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10377" name="Picture 1">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ACC6CFE-3AC8-48FA-A0FC-AE9A95183146}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3D70F1A-C445-42A8-B749-185F59386F1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1222,7 +1225,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="266700" y="219075"/>
-          <a:ext cx="3571875" cy="1028700"/>
+          <a:ext cx="3569493" cy="1038225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1259,20 +1262,20 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>733425</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2640806</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10378" name="Picture 2" descr="Iowa Department of Natural Resources">
+        <xdr:cNvPr id="3" name="Picture 2" descr="Iowa Department of Natural Resources">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9954EC27-2D55-43A3-BE1F-D9C0F028F252}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C928403B-D32B-4B03-BF7F-BDED473DF684}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1295,8 +1298,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5438775" y="161925"/>
-          <a:ext cx="4210050" cy="800100"/>
+          <a:off x="6467475" y="171450"/>
+          <a:ext cx="4202906" cy="790575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1333,7 +1336,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
@@ -1343,10 +1346,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10379" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
+        <xdr:cNvPr id="4" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFDD64F6-E2B4-4660-9C18-BCFBBB16B68E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6B6CA83-FDC9-4AE6-949E-C41289A96AA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1369,8 +1372,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11410950" y="200025"/>
-          <a:ext cx="1152525" cy="962025"/>
+          <a:off x="14001750" y="209550"/>
+          <a:ext cx="1152525" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1701,7 +1704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W1"/>
   <sheetViews>
@@ -1802,7 +1805,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W1"/>
+  <autoFilter ref="A1:W1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -1812,7 +1815,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2">
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -1823,20 +1826,20 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.28515625" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="5" max="5" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="39.5703125" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" customWidth="1"/>
+    <col min="8" max="8" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" customWidth="1"/>
+    <col min="11" max="11" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.7109375" customWidth="1"/>
-    <col min="14" max="14" width="30.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" customWidth="1"/>
+    <col min="14" max="14" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="2:14" ht="33.75" x14ac:dyDescent="0.5">
@@ -1883,7 +1886,7 @@
     <mergeCell ref="B9:N9"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="85" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="45" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
@@ -1892,7 +1895,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E7A02E-1BFE-4AF5-AC7E-7BA54E063585}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -1903,20 +1906,20 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.28515625" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="5" max="5" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="40.28515625" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" customWidth="1"/>
+    <col min="8" max="8" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="40.28515625" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" customWidth="1"/>
+    <col min="11" max="11" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.7109375" customWidth="1"/>
-    <col min="14" max="14" width="40.28515625" customWidth="1"/>
-    <col min="15" max="15" width="4.28515625" customWidth="1"/>
+    <col min="14" max="14" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="2:14" ht="33.75" x14ac:dyDescent="0.5">
@@ -1963,7 +1966,7 @@
     <mergeCell ref="B9:N9"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="85" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="45" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
@@ -1972,7 +1975,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53607111-4F55-4FE9-AC7B-2954921ECDB7}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -1982,20 +1985,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.28515625" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="5" max="5" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="39.5703125" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" customWidth="1"/>
+    <col min="8" max="8" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" customWidth="1"/>
-    <col min="14" max="14" width="30.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" customWidth="1"/>
+    <col min="11" max="11" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" customWidth="1"/>
+    <col min="14" max="14" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="2:14" ht="33.75" x14ac:dyDescent="0.5">
@@ -2024,13 +2028,25 @@
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="E12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B9:N9"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="85" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="45" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
@@ -2039,7 +2055,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet4">
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
@@ -2050,25 +2066,25 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="35.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.7109375" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="35.7109375" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4.7109375" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" customWidth="1"/>
-    <col min="19" max="19" width="6.7109375" style="4" customWidth="1"/>
-    <col min="20" max="20" width="35.7109375" customWidth="1"/>
+    <col min="18" max="18" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="43.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
@@ -2226,12 +2242,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A13:T13"/>
+  <autoFilter ref="A13:T13" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <mergeCells count="1">
     <mergeCell ref="B9:L9"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="31" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
@@ -2240,7 +2256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24EF37EC-8F1F-4285-ADF1-C36CAB26CE14}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
@@ -2251,25 +2267,25 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="35.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.7109375" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="35.7109375" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4.7109375" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" customWidth="1"/>
-    <col min="19" max="19" width="6.7109375" style="4" customWidth="1"/>
-    <col min="20" max="20" width="35.7109375" customWidth="1"/>
+    <col min="18" max="18" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="43.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
@@ -2427,12 +2443,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A13:T13"/>
+  <autoFilter ref="A13:T13" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <mergeCells count="1">
     <mergeCell ref="B9:L9"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="31" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
@@ -2441,7 +2457,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2492,7 +2508,7 @@
       <c r="U1" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update page break preview and headers
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppDev\code\trap-scoring\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Busche\Desktop\apps\code\trap-scoring\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F942B243-8EF1-474C-BC41-00C8BDE17C71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B3AA32-2596-4ED7-83B7-610F823984D3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="18240" windowHeight="7920" tabRatio="623" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="623" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clean Data" sheetId="1" r:id="rId1"/>
     <sheet name="Team-Senior" sheetId="2" r:id="rId2"/>
-    <sheet name="Team-Intermediate" sheetId="14" r:id="rId3"/>
-    <sheet name="Team-Rookie" sheetId="15" r:id="rId4"/>
+    <sheet name="Team-Intermediate" sheetId="17" r:id="rId3"/>
+    <sheet name="Team-Rookie" sheetId="18" r:id="rId4"/>
     <sheet name="Individual-Men" sheetId="4" r:id="rId5"/>
-    <sheet name="Individual-Ladies" sheetId="16" r:id="rId6"/>
+    <sheet name="Individual-Ladies" sheetId="19" r:id="rId6"/>
     <sheet name="Team-Individual-Scores" sheetId="13" r:id="rId7"/>
   </sheets>
   <definedNames>
@@ -26,12 +26,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Individual-Ladies'!$A$13:$T$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Individual-Men'!$A$13:$T$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Team-Individual-Scores'!$A$1:$F$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Team-Intermediate'!$A$1:$P$12</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Team-Rookie'!$A$1:$P$12</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Team-Senior'!$A$1:$P$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Individual-Ladies'!$A$1:$T$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Individual-Men'!$A$1:$T$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Team-Intermediate'!$A$1:$P$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Team-Rookie'!$A$1:$P$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Team-Senior'!$A$1:$P$48</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Clean Data'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="5">'Individual-Ladies'!$1:$13</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="4">'Individual-Men'!$1:$13</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">'Individual-Ladies'!$12:$13</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">'Individual-Men'!$12:$13</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Team-Intermediate'!$12:$12</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Team-Rookie'!$12:$12</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Team-Senior'!$12:$12</definedName>
@@ -520,7 +522,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13F7CE4F-753B-4DDA-9E61-3998DEBE4AFC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A47D108-9D59-4468-94B8-DBA90340F3DB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -594,7 +596,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="Iowa Department of Natural Resources">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63B5BE74-514F-4F18-A16A-605CF8A98D47}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FA1C945-50C3-48C5-A924-F09F651F4A94}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -668,7 +670,7 @@
         <xdr:cNvPr id="4" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6663856E-F654-4EB9-9BDB-1B1ABD809EF8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7A17FA6-167A-431D-A3C2-4901C1D2FF7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -747,7 +749,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E260745-D8AE-4701-9E3B-BD669E90D5CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78AF5AD0-8E13-41A6-852D-6C63849EE66A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -821,7 +823,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="Iowa Department of Natural Resources">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87AA494B-BE5B-4CD1-8DD0-69B92D43E4D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85AACD84-7491-4BA6-8F0E-06D910A640AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -895,7 +897,7 @@
         <xdr:cNvPr id="4" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A1E53A0-3DAF-41EB-99B2-273277619DB4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6C00317-B9D0-4CF2-8A84-6299070B9179}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1201,7 +1203,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3D70F1A-C445-42A8-B749-185F59386F1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2588A2FC-8D28-4B61-97FD-19E88759F9FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1275,7 +1277,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="Iowa Department of Natural Resources">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C928403B-D32B-4B03-BF7F-BDED473DF684}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72A21AEC-80FD-4A54-AE33-257F4FD3D6B7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1349,7 +1351,7 @@
         <xdr:cNvPr id="4" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6B6CA83-FDC9-4AE6-949E-C41289A96AA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C98A8A4-F755-465E-BC96-5A01E682CB66}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1895,7 +1897,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E7A02E-1BFE-4AF5-AC7E-7BA54E063585}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FD8A92-A37C-43F3-BCAE-69A003C55DCE}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -1975,7 +1977,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53607111-4F55-4FE9-AC7B-2954921ECDB7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB9EF0D-358A-4D45-91FE-35268C5E8A07}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -2256,7 +2258,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24EF37EC-8F1F-4285-ADF1-C36CAB26CE14}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8B4FD5-8384-4590-B0B0-08815B8C9CC8}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>

</xml_diff>

<commit_message>
update page breaks and headers
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Busche\Desktop\apps\code\trap-scoring\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppDev\code\trap-scoring\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B3AA32-2596-4ED7-83B7-610F823984D3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A82FB67-819D-4B8F-AB06-F4A321CAB925}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="623" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clean Data" sheetId="1" r:id="rId1"/>
     <sheet name="Team-Senior" sheetId="2" r:id="rId2"/>
-    <sheet name="Team-Intermediate" sheetId="17" r:id="rId3"/>
-    <sheet name="Team-Rookie" sheetId="18" r:id="rId4"/>
+    <sheet name="Team-Intermediate" sheetId="20" r:id="rId3"/>
+    <sheet name="Team-Rookie" sheetId="21" r:id="rId4"/>
     <sheet name="Individual-Men" sheetId="4" r:id="rId5"/>
-    <sheet name="Individual-Ladies" sheetId="19" r:id="rId6"/>
+    <sheet name="Individual-Ladies" sheetId="22" r:id="rId6"/>
     <sheet name="Team-Individual-Scores" sheetId="13" r:id="rId7"/>
   </sheets>
   <definedNames>
@@ -26,11 +26,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Individual-Ladies'!$A$13:$T$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Individual-Men'!$A$13:$T$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Team-Individual-Scores'!$A$1:$F$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">'Individual-Ladies'!$A$1:$T$45</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'Individual-Men'!$A$1:$T$45</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Team-Intermediate'!$A$1:$P$48</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Team-Rookie'!$A$1:$P$48</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Team-Senior'!$A$1:$P$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Individual-Ladies'!$A$1:$T$63</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Individual-Men'!$A$1:$T$63</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Team-Intermediate'!$A$1:$U$71</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Team-Rookie'!$A$1:$U$71</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Team-Senior'!$A$1:$U$71</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Clean Data'!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="5">'Individual-Ladies'!$12:$13</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'Individual-Men'!$12:$13</definedName>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
   <si>
     <t>EventId</t>
   </si>
@@ -318,8 +318,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="190500" y="209550"/>
-          <a:ext cx="3571875" cy="1028700"/>
+          <a:off x="187325" y="209550"/>
+          <a:ext cx="3570288" cy="1028700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -354,15 +354,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1714500</xdr:colOff>
+      <xdr:colOff>404814</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2083593</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>773907</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -392,8 +392,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5362575" y="142875"/>
-          <a:ext cx="4200525" cy="800100"/>
+          <a:off x="4405314" y="190499"/>
+          <a:ext cx="4202906" cy="800100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -427,14 +427,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1757372</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1552575</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2909897</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -466,7 +466,229 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10972800" y="209550"/>
+          <a:off x="9591685" y="209550"/>
+          <a:ext cx="1152525" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190442</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>7141</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>442854</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>83341</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{297FC058-DB3A-4DC9-9EA8-E782BF58A06D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11858567" y="197641"/>
+          <a:ext cx="3574256" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>566680</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>178590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>233305</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>26190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 2" descr="Iowa Department of Natural Resources">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8665F83F-FBAC-4488-8C2E-6866DC9EF641}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16068618" y="178590"/>
+          <a:ext cx="4202906" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>2333</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>7141</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>547639</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>7141</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{407C9BD4-04A0-4D6C-AEF2-E51CD5D85BC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="21254989" y="197641"/>
           <a:ext cx="1152525" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -522,7 +744,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A47D108-9D59-4468-94B8-DBA90340F3DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C1B79AE-34B8-4FD9-BBFA-BD55573C9394}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -581,22 +803,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1714500</xdr:colOff>
+      <xdr:colOff>404814</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2083593</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>773907</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2" descr="Iowa Department of Natural Resources">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FA1C945-50C3-48C5-A924-F09F651F4A94}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89C70E76-0156-4901-9974-4CC7A371F936}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -619,7 +841,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5715000" y="142875"/>
+          <a:off x="4405314" y="190499"/>
           <a:ext cx="4207668" cy="800100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -654,14 +876,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1757372</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1552575</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2909897</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -670,7 +892,7 @@
         <xdr:cNvPr id="4" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7A17FA6-167A-431D-A3C2-4901C1D2FF7F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4490D16-492E-4EFB-85B3-64DF99B5F4C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -693,8 +915,230 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12077700" y="209550"/>
+          <a:off x="9596447" y="209550"/>
           <a:ext cx="1152525" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190442</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>7141</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>442854</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>83341</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30782403-1AE7-44C5-93D2-BC7C85CC9F5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11868092" y="197641"/>
+          <a:ext cx="3576637" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>566680</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>178590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>233305</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>26190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 2" descr="Iowa Department of Natural Resources">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FCCFC8E-A26B-487B-A5EC-FBC7BC35DD36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16082905" y="178590"/>
+          <a:ext cx="4210050" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>2333</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>7141</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>547639</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>7141</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7FF90E4-5F5F-45D0-BE9D-76B45A0F5061}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="21281183" y="197641"/>
+          <a:ext cx="1154906" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -749,7 +1193,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78AF5AD0-8E13-41A6-852D-6C63849EE66A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{338D92AA-6341-4F92-B507-8D0F3F07B997}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -808,22 +1252,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1714500</xdr:colOff>
+      <xdr:colOff>404814</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2083593</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>773907</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2" descr="Iowa Department of Natural Resources">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85AACD84-7491-4BA6-8F0E-06D910A640AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15A47CE8-0182-40D0-ACBA-C01F25AB99DA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -846,7 +1290,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5715000" y="142875"/>
+          <a:off x="4405314" y="190499"/>
           <a:ext cx="4207668" cy="800100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -881,14 +1325,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1757372</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1552575</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2909897</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -897,7 +1341,7 @@
         <xdr:cNvPr id="4" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6C00317-B9D0-4CF2-8A84-6299070B9179}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{336314FE-0E82-4888-A7D9-49128146FAD9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -920,7 +1364,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12077700" y="209550"/>
+          <a:off x="9596447" y="209550"/>
           <a:ext cx="1152525" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -961,22 +1405,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>83342</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161923</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1293018</xdr:colOff>
+      <xdr:colOff>1359691</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>47623</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5307" name="Picture 1">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91423D22-1D39-4317-B4B2-4EC071F78563}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED6F4B72-91F4-4220-B884-EED419E6D54B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -999,8 +1443,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="266700" y="219075"/>
-          <a:ext cx="3571875" cy="1038225"/>
+          <a:off x="333373" y="161923"/>
+          <a:ext cx="3574256" cy="1028700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1034,23 +1478,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1995486</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>142872</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2640806</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>709611</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180972</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5308" name="Picture 2" descr="Iowa Department of Natural Resources">
+        <xdr:cNvPr id="6" name="Picture 5" descr="Iowa Department of Natural Resources">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF068B46-6D03-4233-807D-9BF5E551F93D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3177B6C-9114-437A-8DE5-A8F8C21655EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1073,8 +1517,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5438775" y="171450"/>
-          <a:ext cx="4210050" cy="790575"/>
+          <a:off x="4543424" y="142872"/>
+          <a:ext cx="4202906" cy="800100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1108,23 +1552,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1693076</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161923</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1638300</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2845601</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161923</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5309" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
+        <xdr:cNvPr id="7" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63CAE1DB-76F9-46B7-AF40-4F41090C2E45}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72D5E5B3-23DE-47B5-827C-7C6BBB140D81}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1147,7 +1591,229 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11410950" y="209550"/>
+          <a:off x="9729795" y="161923"/>
+          <a:ext cx="1152525" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>414265</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>111921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1690615</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>188121</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9ED99116-A512-43E3-B971-A06DED17812A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="17130640" y="111921"/>
+          <a:ext cx="3574256" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>2326410</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>92870</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>802409</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>130970</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="Iowa Department of Natural Resources">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{138E4428-0A84-42D4-A0DB-52638D0E5D79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="21340691" y="92870"/>
+          <a:ext cx="4202906" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1785874</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>111921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>57087</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>111921</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38A41606-FE5A-42BC-9E10-EB4C47C29CC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="26527062" y="111921"/>
           <a:ext cx="1152525" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1188,22 +1854,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>83342</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161923</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1293018</xdr:colOff>
+      <xdr:colOff>1359691</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>47623</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2588A2FC-8D28-4B61-97FD-19E88759F9FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77AD06AA-0464-4D30-B8AF-BAAC541546E3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1226,8 +1892,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="266700" y="219075"/>
-          <a:ext cx="3569493" cy="1038225"/>
+          <a:off x="330992" y="161923"/>
+          <a:ext cx="3571874" cy="1028700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1261,23 +1927,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1995486</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>142872</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2640806</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>709611</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180972</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2" descr="Iowa Department of Natural Resources">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72A21AEC-80FD-4A54-AE33-257F4FD3D6B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32878D0B-D165-4AAD-8A6F-F110950419D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1300,8 +1966,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6467475" y="171450"/>
-          <a:ext cx="4202906" cy="790575"/>
+          <a:off x="4538661" y="142872"/>
+          <a:ext cx="4200525" cy="800100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1335,23 +2001,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1693076</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161923</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1638300</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2845601</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161923</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C98A8A4-F755-465E-BC96-5A01E682CB66}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A270960E-CB6E-4B89-839F-F1D7C4F0FB8E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1374,8 +2040,230 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="14001750" y="209550"/>
+          <a:off x="9722651" y="161923"/>
           <a:ext cx="1152525" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>414265</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>111921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1690615</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>188121</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DB5B063-B781-4378-BB79-019E54C842DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="17121115" y="111921"/>
+          <a:ext cx="3571875" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>2326410</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>92870</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>802409</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>130970</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="Iowa Department of Natural Resources">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D3517D4-8D84-4CE0-B1CC-A18F51080566}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="21328785" y="92870"/>
+          <a:ext cx="4200524" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1785874</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>111921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>57087</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>111921</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 5" descr="https://sssfonline.org/wp-content/uploads/2014/03/clayTarget-logo.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B65A8D33-A5FF-4FEB-822D-8AB6EF846314}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="26512774" y="111921"/>
+          <a:ext cx="1147763" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1712,7 +2600,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,16 +2776,22 @@
     <mergeCell ref="B9:N9"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="45" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="76" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="35" max="20" man="1"/>
+  </rowBreaks>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="10" max="70" man="1"/>
+  </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FD8A92-A37C-43F3-BCAE-69A003C55DCE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8DB859-2075-4F1F-B801-CCED18C399E9}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -1968,16 +2862,22 @@
     <mergeCell ref="B9:N9"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="45" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="76" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="35" max="20" man="1"/>
+  </rowBreaks>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="10" max="70" man="1"/>
+  </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB9EF0D-358A-4D45-91FE-35268C5E8A07}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACAEB1E-5166-4F2F-9469-7C993064F06B}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -2030,28 +2930,22 @@
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N12" s="6" t="s">
-        <v>25</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B9:N9"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="45" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="76" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="35" max="20" man="1"/>
+  </rowBreaks>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="10" max="70" man="1"/>
+  </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -2253,12 +3147,18 @@
   <headerFooter>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="32" max="16383" man="1"/>
+  </rowBreaks>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="13" max="62" man="1"/>
+  </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8B4FD5-8384-4590-B0B0-08815B8C9CC8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F3AF09-0935-4B97-AF12-CE1C1B98D7BA}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
@@ -2454,6 +3354,12 @@
   <headerFooter>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="32" max="16383" man="1"/>
+  </rowBreaks>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="13" max="62" man="1"/>
+  </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add tab for all individual scores
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppDev\code\trap-scoring\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A82FB67-819D-4B8F-AB06-F4A321CAB925}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E222A1-2EDF-45B8-A200-1B333A9950B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="623" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="672" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clean Data" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,14 @@
     <sheet name="Individual-Men" sheetId="4" r:id="rId5"/>
     <sheet name="Individual-Ladies" sheetId="22" r:id="rId6"/>
     <sheet name="Team-Individual-Scores" sheetId="13" r:id="rId7"/>
+    <sheet name="Individual-All-Scores" sheetId="24" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Clean Data'!$A$1:$W$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Individual-All-Scores'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Individual-Ladies'!$A$13:$T$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Individual-Men'!$A$13:$T$13</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Team-Individual-Scores'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Team-Individual-Scores'!$A$1:$E$1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'Individual-Ladies'!$A$1:$T$63</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Individual-Men'!$A$1:$T$63</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Team-Intermediate'!$A$1:$U$71</definedName>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="37">
   <si>
     <t>EventId</t>
   </si>
@@ -154,9 +156,6 @@
   </si>
   <si>
     <t>IndTotal</t>
-  </si>
-  <si>
-    <t>TeamTotal</t>
   </si>
 </sst>
 </file>
@@ -2600,7 +2599,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3366,13 +3365,71 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B742CF68-D3E0-46BD-91E7-1F9358E89E85}">
+  <dimension ref="A1:U1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
@@ -3397,7 +3454,7 @@
         <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>

</xml_diff>